<commit_message>
add updated references after the final defense
</commit_message>
<xml_diff>
--- a/P4_01_rapport_analyse.xlsx
+++ b/P4_01_rapport_analyse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33613\Documents\Formation DEV WEB\004_projet_4\P4_ZHANG_Jing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C6E80-80CA-4AE9-881C-9DBEBC3D63FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1991E2E-9CD6-41E0-BBDB-245ABB4BA97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="113">
   <si>
     <t>Catégorie</t>
   </si>
@@ -60,24 +60,9 @@
     <t>Responsive design</t>
   </si>
   <si>
-    <t>2.4.4 Link Purpose (In Context) (Level A)</t>
-  </si>
-  <si>
     <t>Supprimer les mots-clés cachés.</t>
   </si>
   <si>
-    <t>3.1.1 Language of Page 
-(Level A)</t>
-  </si>
-  <si>
-    <t>1.4.3 Contrast (Minimum) 
-(Level AA)</t>
-  </si>
-  <si>
-    <t>1.4.3: Contrast
-(Minimum)</t>
-  </si>
-  <si>
     <t>Supprimer ces liens</t>
   </si>
   <si>
@@ -87,14 +72,6 @@
     <t>Remplacer "page 2&gt;" par "Contact"</t>
   </si>
   <si>
-    <t>1.3.1 Info and Relationships (Level A)
-2.4.1 Bypass Blocks (Level A)
-2.4.6 Headings and Labels (Level AA)</t>
-  </si>
-  <si>
-    <t>1.1.1 Non-text Content (Level A)</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -117,15 +94,6 @@
   </si>
   <si>
     <t>Préciser les étiquettes de texte pour chaque champs avec l'élément &lt;label&gt;.</t>
-  </si>
-  <si>
-    <t>1.1.1 Non-text Content (Level A)
-1.3.1 Info and Relationships (Level A)
-2.4.6 Headings and Labels (Level AA)
-3.3.2 Labels or Instructions (Level A)</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>Menu "page 2" dans la barre de navigation</t>
@@ -233,12 +201,6 @@
   </si>
   <si>
     <t>Mettre les liens et les boutons avec le "focus"</t>
-  </si>
-  <si>
-    <t>1.1.1: Non-text
-Content
-2.1.1:
-Keyboard</t>
   </si>
   <si>
     <r>
@@ -327,18 +289,6 @@
     <t>Balises sémantiques</t>
   </si>
   <si>
-    <t>Fichier HTML &amp; CSS non-optimisés</t>
-  </si>
-  <si>
-    <t>Certains balises ont des nommages trop long dans le fichier htmls
-Certains attributs ne sont pas optimisés ou utilisés dans les fichiers css.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avoir une convention de nommage BEM pour les fichiers htmls
-Supprimer les balises non-utilisés et optimser les attribus dans les fichiers css.
-</t>
-  </si>
-  <si>
     <t>Action recommandée</t>
   </si>
   <si>
@@ -382,32 +332,122 @@
 *exécution différée defer  &lt;script defer src=""&gt;&lt;/script&gt;. </t>
   </si>
   <si>
-    <t>Supprimer les fichiers javascript ou css non-utiliser</t>
-  </si>
-  <si>
-    <t>Mettre à jour la libraire Jquery utiliser</t>
-  </si>
-  <si>
     <t>La balise "alt" des images n'est pas bien renseignée</t>
   </si>
   <si>
-    <t>Identifier les fichiers javascript ou css non-utilisés</t>
-  </si>
-  <si>
-    <t>Vérifrier la mise à jour de la libraire Jquery</t>
-  </si>
-  <si>
     <t>ETAPE 2</t>
   </si>
   <si>
     <t>ETAPE 3</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/crawling/special-tags?hl=fr
+https://developer.mozilla.org/fr/docs/Web/HTML/Element/meta
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578344-creez-votre-machine-a-contenu</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5603511-nouez-des-partenariats</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/NOTE-UNDERSTANDING-WCAG20-fr-20110706/visual-audio-contrast7.html
+https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/visual-audio-contrast-contrast.html</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/WCAG21/#language-of-page</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site
+https://developer.mozilla.org/fr/docs/Web/HTML/Element/Img</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055226-pensez-mobile-first</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055236-parametrez-le-cache-navigateur</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Learn/Accessibility/HTML</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/WCAG21/#link-purpose-in-context</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/WCAG21/#info-and-relationships
+https://www.w3.org/TR/WCAG21/#headings-and-labels
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/WCAG21/#labels-or-instructions</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941263-creez-des-designs-visuels-accessibles</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941114-testez-votre-contenu-a-laide-de-technologies-dassistance
+https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941406-rendez-les-interactions-sur-le-site-accessibles
+https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist
+https://www.w3.org/TR/WCAG21/#keyboard
+https://www.w3.org/TR/WCAG21/#text-alternatives</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/NOTE-UNDERSTANDING-WCAG20-fr-20110706/consistent-behavior-consistent-locations.html
+https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941406-rendez-les-interactions-sur-le-site-accessibles</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
+  </si>
+  <si>
+    <t>Identifier les fichiers javascript ou css ou html non-utilisés</t>
+  </si>
+  <si>
+    <t>Supprimer les fichiers javascript ou css non-utiliser
+Avoir une convention de nommage BEM pour les fichiers htmls
+Supprimer les balises non-utilisés et optimser les attribus dans les fichiers css.</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site
+https://www.codeur.com/tuto/css/ameliorer-vitesse-site/</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5604431-installez-les-bons-outils
+https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055216-ameliorez-votre-crawlabilite-pour-une-meilleure-indexation
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578349-analysez-vos-kpis-grace-a-google-analytics
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578350-suivez-votre-progression-grace-a-google-search-console</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site
+https://www.w3.org/TR/WCAG21/#link-purpose-in-context
+https://www.redacteur.com/blog/seo-liens-penalisant-google/</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Learn/HTML/Multimedia_and_embedding/Responsive_images
+https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -449,10 +489,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -537,10 +584,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -563,14 +611,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,9 +622,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,9 +635,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,14 +644,18 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -839,23 +879,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="39.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="43.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46.54296875" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.90625" style="3" customWidth="1"/>
     <col min="8" max="26" width="10.54296875" style="3" customWidth="1"/>
     <col min="27" max="16384" width="11.26953125" style="3"/>
@@ -875,13 +915,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -903,96 +943,96 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>12</v>
+        <v>73</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>92</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
+        <v>73</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1000,530 +1040,486 @@
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>11</v>
+      <c r="F6" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="128.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>27</v>
+        <v>73</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="9" spans="1:26" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>27</v>
+        <v>73</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>110</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>22</v>
+        <v>73</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="26" t="s">
+      <c r="A12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>76</v>
+      <c r="G12" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="212.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>22</v>
+      <c r="B13" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="15" t="s">
+      <c r="C16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>76</v>
+      <c r="G18" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+    <row r="19" spans="1:7" s="4" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>22</v>
+      <c r="B19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>22</v>
+      <c r="C24" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>22</v>
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="16" t="s">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="27" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1534,8 +1530,8 @@
     <row r="36" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2494,11 +2490,30 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:Z1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/NOTE-UNDERSTANDING-WCAG20-fr-20110706/visual-audio-contrast7.html" xr:uid="{33107B8E-E0B2-4828-B199-99F2BE088F60}"/>
+    <hyperlink ref="F5" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Learn/HTML/Multimedia_and_embedding/Responsive_images" xr:uid="{D85B5DC9-861B-441C-A95A-FDF93387DBEC}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{6F8AA6C7-120F-4BC1-9EFF-FF9EC22E432C}"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://www.redacteur.com/blog/seo-liens-penalisant-google/" xr:uid="{FEF136F6-5ED4-4332-910B-BB82B875F162}"/>
+    <hyperlink ref="F4" r:id="rId5" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html" xr:uid="{F817B610-964D-4B49-A4E7-433C3B0F3018}"/>
+    <hyperlink ref="F16" r:id="rId6" xr:uid="{8E03FE55-4F5B-42B3-9AE1-CBA366334B11}"/>
+    <hyperlink ref="F26" r:id="rId7" xr:uid="{942A6F2E-7F2A-428A-8153-11A8D6C716C4}"/>
+    <hyperlink ref="F25" r:id="rId8" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site" xr:uid="{20821E9E-DDCF-4868-A86D-A4C5F54D6591}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{6FA16197-5584-4068-BAF5-1ABA269CE9C9}"/>
+    <hyperlink ref="F23" r:id="rId10" xr:uid="{12D9C2B5-7F35-4D72-9D99-36BC5ED1253F}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{9D3DA978-F077-409D-897F-67646D0D9DE8}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{DA53FF98-C800-4EC6-BDC8-7FF332E13DEA}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{10B8D19C-82E2-4D17-9C3A-E1377CBA0E95}"/>
+    <hyperlink ref="F17" r:id="rId14" location="link-purpose-in-context" xr:uid="{1FE7EF8E-3BD3-4DD0-813F-F75BBE4894A2}"/>
+    <hyperlink ref="F19" r:id="rId15" location="labels-or-instructions" xr:uid="{16679E6A-54CC-46D8-A30B-98DF42B9F666}"/>
+    <hyperlink ref="F20" r:id="rId16" xr:uid="{923BF41C-A4E5-4A20-BA3D-8AA9016429A3}"/>
+    <hyperlink ref="F21" r:id="rId17" display="https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941406-rendez-les-interactions-sur-le-site-accessibles" xr:uid="{57511C6E-2783-45D8-8938-A95A44E41E76}"/>
+    <hyperlink ref="F22" r:id="rId18" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages" xr:uid="{7A5A6F44-BF23-49BF-A43F-210DDD4A8B2F}"/>
+    <hyperlink ref="F24" r:id="rId19" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site_x000a_" xr:uid="{2ED34EF6-A1F7-4D6D-827F-495655AA8F6B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>